<commit_message>
unstable MonthlyMarsReport -> Agent Summary
</commit_message>
<xml_diff>
--- a/automated_sla_tool/settings/report_settings.xlsx
+++ b/automated_sla_tool/settings/report_settings.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Ameren</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Carlson</t>
   </si>
   <si>
-    <t>Universal Serv</t>
-  </si>
-  <si>
     <t>Nordstrom</t>
   </si>
   <si>
@@ -144,6 +141,12 @@
   </si>
   <si>
     <t>BBA Aviation</t>
+  </si>
+  <si>
+    <t>ClearwaterPaper</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -502,31 +505,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>2029</v>
@@ -559,7 +562,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>7508</v>
@@ -581,7 +584,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>7512</v>
@@ -603,7 +606,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <v>7516</v>
@@ -631,7 +634,7 @@
         <v>7521</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -647,18 +650,18 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>7524</v>
       </c>
-      <c r="C13" s="3" t="b">
-        <v>0</v>
+      <c r="C13" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>7527</v>
@@ -669,7 +672,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>7539</v>
@@ -680,7 +683,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>7543</v>
@@ -691,7 +694,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>7544</v>
@@ -702,7 +705,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>7545</v>
@@ -713,7 +716,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>7547</v>
@@ -724,7 +727,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20">
         <v>7548</v>
@@ -735,7 +738,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21">
         <v>7549</v>
@@ -746,7 +749,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22">
         <v>7551</v>
@@ -757,7 +760,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23">
         <v>7553</v>
@@ -768,7 +771,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24">
         <v>7557</v>
@@ -779,7 +782,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25">
         <v>7558</v>
@@ -790,7 +793,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26">
         <v>7561</v>
@@ -801,7 +804,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27">
         <v>7567</v>
@@ -812,7 +815,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28">
         <v>7576</v>
@@ -823,7 +826,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29">
         <v>7577</v>
@@ -834,7 +837,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30">
         <v>7578</v>
@@ -845,7 +848,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31">
         <v>7579</v>
@@ -856,7 +859,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32">
         <v>7589</v>
@@ -867,7 +870,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33">
         <v>7595</v>
@@ -878,7 +881,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34">
         <v>7591</v>
@@ -889,7 +892,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35">
         <v>7592</v>
@@ -900,7 +903,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36">
         <v>7593</v>
@@ -911,10 +914,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>7593</v>
+        <v>7594</v>
       </c>
       <c r="C37" s="3" t="b">
         <v>0</v>

</xml_diff>